<commit_message>
Adding some changes in code
</commit_message>
<xml_diff>
--- a/src/main/resources/stations.xlsx
+++ b/src/main/resources/stations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Erail_OrangeAutomationFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB20BD93-A823-4801-8F85-A03D970CED53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29542129-3926-473A-9F73-01816AC4363E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
   <si>
     <t>Denduluru
 DEL</t>
@@ -391,7 +391,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:XFD1048576"/>
+      <selection activeCell="K9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Waits utils and Optimized the scripts with the same.
</commit_message>
<xml_diff>
--- a/src/main/resources/stations.xlsx
+++ b/src/main/resources/stations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Erail_OrangeAutomationFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29542129-3926-473A-9F73-01816AC4363E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6155FBE7-8221-41A8-BDB1-4EB5FFB942F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="4">
   <si>
     <t>Denduluru
 DEL</t>
@@ -391,7 +391,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="A1:XFD1048576"/>
+      <selection activeCell="Q5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>